<commit_message>
reformat architecture and update the tester nodes
</commit_message>
<xml_diff>
--- a/opset_20/NVIDIA - TensorRT/report_TensorrtExecutionProvider.xlsx
+++ b/opset_20/NVIDIA - TensorRT/report_TensorrtExecutionProvider.xlsx
@@ -41,12 +41,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
+        <fgColor rgb="00DEDEDE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DEDEDE"/>
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -816,10 +816,14 @@
           <t>TensorrtExecutionProvider</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr"/>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>FAIL session creation: [ONNXRuntimeError] : 1 : FAIL : TensorRT EP failed to create engine from network for fused node: TensorrtExecutionProvider_TRTKernel_graph_bernoulli_graph_3158215355511095402_0_0</t>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>TensorrtExecutionProvider</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -951,7 +955,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1147,7 @@
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr"/>
-      <c r="D24" s="4" t="inlineStr">
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>UNKNOWN (no Node event)</t>
         </is>
@@ -1255,7 +1259,7 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1341,7 @@
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr"/>
-      <c r="D33" s="3" t="inlineStr">
+      <c r="D33" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", DequantizeLinear, "", -1) : ("x": tensor(uint8),"x_scale": tensor(float),"x_zero_point": tensor(uint8),) -&gt; ("y": tensor(float),) , Error Unrecognized attribute: block_size for operator DequantizeLinear</t>
         </is>
@@ -1795,7 +1799,7 @@
         </is>
       </c>
       <c r="C54" s="1" t="inlineStr"/>
-      <c r="D54" s="3" t="inlineStr">
+      <c r="D54" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", GroupNormalization, "", -1) : ("X": tensor(float),"scale": tensor(float),"B": tensor(float),) -&gt; ("Y": tensor(float),) , Error Unrecognized attribute: stash_type for operator GroupNormalization</t>
         </is>
@@ -1819,7 +1823,7 @@
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1845,7 @@
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1971,7 @@
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr"/>
-      <c r="D62" s="3" t="inlineStr">
+      <c r="D62" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ImageDecoder(20) node with name ''</t>
         </is>
@@ -2541,7 +2545,7 @@
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2567,7 @@
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3315,7 @@
       </c>
       <c r="D123" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3403,7 @@
       </c>
       <c r="D127" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -3547,7 +3551,7 @@
         </is>
       </c>
       <c r="C134" s="1" t="inlineStr"/>
-      <c r="D134" s="3" t="inlineStr">
+      <c r="D134" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">FAIL session creation: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Exception during initialization: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\core\providers\tensorrt\tensorrt_execution_provider.cc:2276 onnxruntime::TensorrtExecutionProvider::GetSupportedList graph_build.Resolve().IsOK() was false. 
 </t>
@@ -3566,7 +3570,7 @@
         </is>
       </c>
       <c r="C135" s="1" t="inlineStr"/>
-      <c r="D135" s="4" t="inlineStr">
+      <c r="D135" s="3" t="inlineStr">
         <is>
           <t>UNKNOWN (no Node event)</t>
         </is>
@@ -3612,7 +3616,7 @@
       </c>
       <c r="D137" s="2" t="inlineStr">
         <is>
-          <t>SUCCESS WITH FALLBACK</t>
+          <t>SUCCESS (via decomposition)</t>
         </is>
       </c>
     </row>
@@ -3628,7 +3632,7 @@
         </is>
       </c>
       <c r="C138" s="1" t="inlineStr"/>
-      <c r="D138" s="3" t="inlineStr">
+      <c r="D138" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">FAIL session creation: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Exception during initialization: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\core\providers\tensorrt\tensorrt_execution_provider.cc:2276 onnxruntime::TensorrtExecutionProvider::GetSupportedList graph_build.Resolve().IsOK() was false. 
 </t>
@@ -4065,7 +4069,7 @@
         </is>
       </c>
       <c r="C158" s="1" t="inlineStr"/>
-      <c r="D158" s="3" t="inlineStr">
+      <c r="D158" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">FAIL session creation: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Exception during initialization: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\core\providers\tensorrt\tensorrt_execution_provider.cc:2276 onnxruntime::TensorrtExecutionProvider::GetSupportedList graph_build.Resolve().IsOK() was false. 
 </t>
@@ -4172,7 +4176,7 @@
         </is>
       </c>
       <c r="C163" s="1" t="inlineStr"/>
-      <c r="D163" s="3" t="inlineStr">
+      <c r="D163" s="4" t="inlineStr">
         <is>
           <t>FAIL run: [ONNXRuntimeError] : 2 : INVALID_ARGUMENT : Non-zero status code returned while running BiasSplitGelu node. Name:'' Status Message: hidden size should be 2560, 5120, 6144, 10240 or 12288, got 12</t>
         </is>
@@ -4344,7 +4348,7 @@
         </is>
       </c>
       <c r="C171" s="1" t="inlineStr"/>
-      <c r="D171" s="3" t="inlineStr">
+      <c r="D171" s="4" t="inlineStr">
         <is>
           <t>FAIL (skipped: known crash)</t>
         </is>
@@ -4406,7 +4410,7 @@
         </is>
       </c>
       <c r="C174" s="1" t="inlineStr"/>
-      <c r="D174" s="3" t="inlineStr">
+      <c r="D174" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 10 : INVALID_GRAPH : This is an invalid model. In Node, ("", com.microsoft.DecoderMaskedSelfAttention, "", -1) : ("X": tensor(float),) -&gt; ("Y": tensor(float),) , Error No Op registered for com.microsoft.DecoderMaskedSelfAttention with domain_version of 20</t>
         </is>
@@ -4424,7 +4428,7 @@
         </is>
       </c>
       <c r="C175" s="1" t="inlineStr"/>
-      <c r="D175" s="3" t="inlineStr">
+      <c r="D175" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for DequantizeBFP(1) node with name ''</t>
         </is>
@@ -4786,7 +4790,7 @@
         </is>
       </c>
       <c r="C192" s="1" t="inlineStr"/>
-      <c r="D192" s="3" t="inlineStr">
+      <c r="D192" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for GemmFastGelu(1) node with name ''</t>
         </is>
@@ -5020,7 +5024,7 @@
         </is>
       </c>
       <c r="C203" s="1" t="inlineStr"/>
-      <c r="D203" s="3" t="inlineStr">
+      <c r="D203" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">FAIL run: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Non-zero status code returned while running MatMulFpQ4 node. Name:'' Status Message: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\contrib_ops\cpu\matmul_fpq4.cc:55 onnxruntime::contrib::MatMulFpQ4::Compute buf_size &gt; 0 was false. Operator MatMulFpQ4 not yet supported on this hardware platform.
 </t>
@@ -5149,7 +5153,7 @@
         </is>
       </c>
       <c r="C209" s="1" t="inlineStr"/>
-      <c r="D209" s="3" t="inlineStr">
+      <c r="D209" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for MulInteger(1) node with name ''</t>
         </is>
@@ -5233,7 +5237,7 @@
         </is>
       </c>
       <c r="C213" s="1" t="inlineStr"/>
-      <c r="D213" s="3" t="inlineStr">
+      <c r="D213" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for NhwcConv(1) node with name ''</t>
         </is>
@@ -5555,7 +5559,7 @@
         </is>
       </c>
       <c r="C228" s="1" t="inlineStr"/>
-      <c r="D228" s="3" t="inlineStr">
+      <c r="D228" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QLinearReduceMean(1) node with name ''</t>
         </is>
@@ -5763,7 +5767,7 @@
         </is>
       </c>
       <c r="C238" s="1" t="inlineStr"/>
-      <c r="D238" s="3" t="inlineStr">
+      <c r="D238" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for QuantizeBFP(1) node with name ''</t>
         </is>
@@ -5869,7 +5873,7 @@
         </is>
       </c>
       <c r="C243" s="1" t="inlineStr"/>
-      <c r="D243" s="3" t="inlineStr">
+      <c r="D243" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for ReduceSumInteger(1) node with name ''</t>
         </is>
@@ -6019,7 +6023,7 @@
         </is>
       </c>
       <c r="C250" s="1" t="inlineStr"/>
-      <c r="D250" s="3" t="inlineStr">
+      <c r="D250" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">FAIL session creation: [ONNXRuntimeError] : 6 : RUNTIME_EXCEPTION : Exception during initialization: C:\Users\COCO\onnxruntime_tensorrt\onnxruntime\core\providers\tensorrt\tensorrt_execution_provider.cc:2276 onnxruntime::TensorrtExecutionProvider::GetSupportedList graph_build.Resolve().IsOK() was false. 
 </t>
@@ -6104,7 +6108,7 @@
         </is>
       </c>
       <c r="C254" s="1" t="inlineStr"/>
-      <c r="D254" s="3" t="inlineStr">
+      <c r="D254" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Snpe(1) node with name ''</t>
         </is>
@@ -6188,7 +6192,7 @@
         </is>
       </c>
       <c r="C258" s="1" t="inlineStr"/>
-      <c r="D258" s="3" t="inlineStr">
+      <c r="D258" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for TorchEmbedding(1) node with name ''</t>
         </is>
@@ -6272,7 +6276,7 @@
         </is>
       </c>
       <c r="C262" s="1" t="inlineStr"/>
-      <c r="D262" s="3" t="inlineStr">
+      <c r="D262" s="4" t="inlineStr">
         <is>
           <t>FAIL session creation: [ONNXRuntimeError] : 9 : NOT_IMPLEMENTED : Could not find an implementation for Unique(1) node with name ''</t>
         </is>
@@ -6345,10 +6349,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C2" t="n">
-        <v>88.2</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="3">
@@ -6436,10 +6440,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>8.4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -6450,7 +6454,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-08-29 10:45:23</t>
+          <t>2025-11-18 14:38:03</t>
         </is>
       </c>
     </row>

</xml_diff>